<commit_message>
Created Crystals and Oscillators library
</commit_message>
<xml_diff>
--- a/Altium Parts.xlsx
+++ b/Altium Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russe\Repositories\MIL\MIL-Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC8AD57-BEEB-43B7-898D-2CCCB2BC7E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C6B5CA-E210-449C-B8B7-FCA8A7839D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{78817FF2-1CC3-4A74-8C91-2AFFF0842C3F}"/>
+    <workbookView xWindow="28680" yWindow="960" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{78817FF2-1CC3-4A74-8C91-2AFFF0842C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome!" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="221">
   <si>
     <t>Capacitance</t>
   </si>
@@ -801,23 +801,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -905,6 +888,23 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -982,18 +982,18 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}" name="Table13" displayName="Table13" ref="A1:F12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}" name="Table13" displayName="Table13" ref="A1:F12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:F12" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
     <sortCondition ref="A1:A12"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E2BB1AD3-36C9-4D80-8A78-E46D0D28B43D}" name="Resistance" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{67EED117-D01D-4FE8-BB40-D7D8F55BAB48}" name="Tolerance" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{F1269AFE-5CA5-4F00-93B8-6023E945504D}" name="Package" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{A4374340-1758-433F-80B6-83ABF6D97E11}" name="Wattage" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{7C53E4E9-C23D-4482-9A46-441AB8A4E1B1}" name="Part Number" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{BD8216A4-1B75-4738-A589-0D33231AD075}" name="Description" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{E2BB1AD3-36C9-4D80-8A78-E46D0D28B43D}" name="Resistance" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{67EED117-D01D-4FE8-BB40-D7D8F55BAB48}" name="Tolerance" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{F1269AFE-5CA5-4F00-93B8-6023E945504D}" name="Package" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A4374340-1758-433F-80B6-83ABF6D97E11}" name="Wattage" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7C53E4E9-C23D-4482-9A46-441AB8A4E1B1}" name="Part Number" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{BD8216A4-1B75-4738-A589-0D33231AD075}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1047,22 +1047,23 @@
     <sortCondition ref="B2:B25"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{CE9E315A-1702-4F78-8ECF-1DA1A2B792AA}" name="Added to Altium?" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{D5AE5A29-FEF0-4556-97F0-002479587894}" name="Series / Family" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{8673F73F-EA18-4F48-837C-C3D933082CD8}" name="Number Pins" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{F61E1994-58CD-4ECF-A835-1786BECF70C2}" name="Gender (plug/port)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{ADD992CB-74CD-4839-9C1F-4CA1C98DDDE6}" name="Part Number" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{E04857DF-CEB1-4D64-87C3-2580C252E44F}" name="Description" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{DAAED122-6C39-41BF-BCC4-71CD183DA6BB}" name="Mating Connector Part Number" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{CE9E315A-1702-4F78-8ECF-1DA1A2B792AA}" name="Added to Altium?" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{D5AE5A29-FEF0-4556-97F0-002479587894}" name="Series / Family" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{8673F73F-EA18-4F48-837C-C3D933082CD8}" name="Number Pins" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{F61E1994-58CD-4ECF-A835-1786BECF70C2}" name="Gender (plug/port)" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{ADD992CB-74CD-4839-9C1F-4CA1C98DDDE6}" name="Part Number" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{E04857DF-CEB1-4D64-87C3-2580C252E44F}" name="Description" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{DAAED122-6C39-41BF-BCC4-71CD183DA6BB}" name="Mating Connector Part Number" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{43F12269-0E76-48CC-8091-7DF9E8B2B894}" name="Table4" displayName="Table4" ref="B2:G1048576" totalsRowShown="0">
-  <autoFilter ref="B2:G1048576" xr:uid="{43F12269-0E76-48CC-8091-7DF9E8B2B894}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{43F12269-0E76-48CC-8091-7DF9E8B2B894}" name="XTALs_and_XOSCs" displayName="XTALs_and_XOSCs" ref="A1:G1048575" totalsRowShown="0">
+  <autoFilter ref="A1:G1048575" xr:uid="{43F12269-0E76-48CC-8091-7DF9E8B2B894}"/>
+  <tableColumns count="7">
+    <tableColumn id="7" xr3:uid="{D0EBBD8D-51DB-4E67-899C-2B8142CB6CCB}" name="Added to Altium?"/>
     <tableColumn id="1" xr3:uid="{765BC975-3EE7-469C-9333-E1FCDABB603D}" name="Frequency"/>
     <tableColumn id="2" xr3:uid="{66DD91D2-5F51-49CF-92CF-17CDB97E3CD8}" name="Type"/>
     <tableColumn id="3" xr3:uid="{228CF721-7ED2-425C-9E3B-C355B3C6E7DB}" name="Load Capacitance"/>
@@ -1075,7 +1076,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}" name="Table5" displayName="Table5" ref="B2:G8" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}" name="Table5" displayName="Table5" ref="B2:G8" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="B2:G8" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3176E398-8316-4079-97C6-E10CED1CC775}" name="Type"/>
@@ -1090,20 +1091,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}" name="Table6" displayName="Table6" ref="A3:D6" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}" name="Table6" displayName="Table6" ref="A3:D6" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A3:D6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{29766E43-A003-4F30-8FBC-98197408FA6D}" name="Part Number" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{9E0E83BD-C619-4B71-B8D8-093D6B07D9D5}" name="Package" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{6C643D04-D582-419C-9C7F-1B57D4315CFE}" name="Resistance" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{67D14711-9F21-4BBC-9182-15BB5F898016}" name="Description" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{29766E43-A003-4F30-8FBC-98197408FA6D}" name="Part Number" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{9E0E83BD-C619-4B71-B8D8-093D6B07D9D5}" name="Package" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{6C643D04-D582-419C-9C7F-1B57D4315CFE}" name="Resistance" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{67D14711-9F21-4BBC-9182-15BB5F898016}" name="Description" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}" name="Table7" displayName="Table7" ref="B2:G9" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}" name="Table7" displayName="Table7" ref="B2:G9" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="B2:G9" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5D9981C8-F221-4013-A9BA-4E5BF3474E5D}" name="Trip Current"/>
@@ -1130,13 +1131,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}" name="Table10" displayName="Table10" ref="A1:D11" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}" name="Table10" displayName="Table10" ref="A1:D11" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:D11" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EBC427FC-C649-421F-A511-F4C6E090217A}" name="Inductance" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{57FAF0ED-182E-4A05-89A5-EE5FE9CF2C31}" name="Package" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{5B4ACDCC-FB26-4063-91C8-D6D43ABD7134}" name="Part Number" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{CFE06357-AAEA-49E4-8ED8-14478316C7C8}" name="Description" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{EBC427FC-C649-421F-A511-F4C6E090217A}" name="Inductance" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{57FAF0ED-182E-4A05-89A5-EE5FE9CF2C31}" name="Package" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{5B4ACDCC-FB26-4063-91C8-D6D43ABD7134}" name="Part Number" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{CFE06357-AAEA-49E4-8ED8-14478316C7C8}" name="Description" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1148,7 +1149,7 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{727DF6C0-6BC9-4CBC-ACBD-F7D7801F3DED}" name="Color"/>
     <tableColumn id="6" xr3:uid="{2F89F121-2031-4E76-8B64-C6BE1AC4E5A7}" name="Mount Type"/>
-    <tableColumn id="2" xr3:uid="{59EEDA5E-A95B-4620-BC5E-79C5C5FB8AFC}" name="Package" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{59EEDA5E-A95B-4620-BC5E-79C5C5FB8AFC}" name="Package" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{95A3DF17-FA71-419C-9869-87ACAC774187}" name="Dome"/>
     <tableColumn id="4" xr3:uid="{30ACC022-FAF3-44FA-97E2-DA5C989B54D7}" name="Part Number"/>
     <tableColumn id="5" xr3:uid="{BDED051F-FA40-461B-85BB-40EDC316E70C}" name="Description"/>
@@ -3010,88 +3011,163 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EC580B-30DF-4B7B-9130-28D1AB04F48B}">
-  <dimension ref="A2:G4"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
     <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
     <col min="4" max="4" width="17.90625" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" customWidth="1"/>
     <col min="6" max="6" width="30.36328125" customWidth="1"/>
     <col min="7" max="7" width="46.54296875" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" hidden="1"/>
+    <col min="9" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
         <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G4" t="s">
         <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added buzzer and 100ohm resistor
</commit_message>
<xml_diff>
--- a/Altium Parts.xlsx
+++ b/Altium Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russe\Repositories\MIL\MIL-Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AF7EC3-F122-408C-89FC-B3F0B20F1655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48AB737-AB46-47AD-B6E2-0727066BB290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="5" activeTab="10" xr2:uid="{78817FF2-1CC3-4A74-8C91-2AFFF0842C3F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="12" xr2:uid="{78817FF2-1CC3-4A74-8C91-2AFFF0842C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome!" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="246">
   <si>
     <t>Capacitance</t>
   </si>
@@ -777,6 +777,21 @@
   </si>
   <si>
     <t>Default mount hole</t>
+  </si>
+  <si>
+    <t>Buzzer (Passive)</t>
+  </si>
+  <si>
+    <t>AI-1223-TWT-3V-2-R</t>
+  </si>
+  <si>
+    <t>Buzzers Indicator, Internally Driven Electromechanical/Magnetic 3 V 30mA 2.3kHz 82dB @ 3V, 10cm Through Hole PC Pins</t>
+  </si>
+  <si>
+    <t>RC0603FR-07100RL</t>
+  </si>
+  <si>
+    <t>RES 100 OHM 1% 1/10W 0603</t>
   </si>
 </sst>
 </file>
@@ -867,54 +882,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="57">
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -927,67 +919,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
           <xfpb:DXFComplement i="0"/>
@@ -1003,49 +941,27 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1057,9 +973,64 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1073,6 +1044,37 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
     </dxf>
     <dxf>
       <fill>
@@ -1096,6 +1098,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1199,7 +1216,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{7B88261C-6B3D-4539-9169-7D9FC231B64A}" name="Misc" displayName="Misc" ref="A1:D13" totalsRowShown="0">
   <autoFilter ref="A1:D13" xr:uid="{7B88261C-6B3D-4539-9169-7D9FC231B64A}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{6C04560D-813B-4E79-B81B-87E653E3F958}" name="Added to Altium?" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{6C04560D-813B-4E79-B81B-87E653E3F958}" name="Added to Altium?" dataDxfId="24"/>
     <tableColumn id="1" xr3:uid="{07652CF2-D7CA-452D-A87D-CEBA35FEC12A}" name="Function"/>
     <tableColumn id="2" xr3:uid="{A9FCB299-A552-4123-B45A-F31F0DC5BB9B}" name="Part Number"/>
     <tableColumn id="3" xr3:uid="{2F50D30B-F60A-4BAF-AE6D-0A3909047904}" name="Description"/>
@@ -1209,49 +1226,49 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9DA4F768-7F47-4563-8367-8C9704917FC2}" name="MCUs" displayName="MCUs" ref="A1:J11" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9DA4F768-7F47-4563-8367-8C9704917FC2}" name="MCUs" displayName="MCUs" ref="A1:J11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:J11" xr:uid="{9DA4F768-7F47-4563-8367-8C9704917FC2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
     <sortCondition ref="B1:B11"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="7" xr3:uid="{B7904B75-EB47-4AE0-AC16-835BCD406E73}" name="Added to Altium?" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{0881C807-AE0D-4E97-942D-F1BB4BC72740}" name="Name" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{FF11C1E0-268B-4AB9-A529-8334EF2C69FD}" name="# GPIO" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{55162BE7-C291-4B9F-ABE8-A7DE102A5A2F}" name="UART" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{12871EC5-67F1-442C-B9F6-E715FA2B13DA}" name="SPI" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{0676FDA2-81C4-49A9-A3D1-DEE7F28D8014}" name="I2C" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{4D86DECE-60FC-46A0-B57F-AB144D9C1459}" name="PWM" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{F498CA82-C855-4B59-BFFB-E076763E2C7B}" name="USB" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{1C8B55E3-7B48-484B-9DEC-D60D33855BF8}" name="Part Number" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{EB01044E-239A-43EB-B0C2-1F87DDB54160}" name="Description" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{B7904B75-EB47-4AE0-AC16-835BCD406E73}" name="Added to Altium?" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{0881C807-AE0D-4E97-942D-F1BB4BC72740}" name="Name" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{FF11C1E0-268B-4AB9-A529-8334EF2C69FD}" name="# GPIO" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{55162BE7-C291-4B9F-ABE8-A7DE102A5A2F}" name="UART" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{12871EC5-67F1-442C-B9F6-E715FA2B13DA}" name="SPI" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{0676FDA2-81C4-49A9-A3D1-DEE7F28D8014}" name="I2C" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{4D86DECE-60FC-46A0-B57F-AB144D9C1459}" name="PWM" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{F498CA82-C855-4B59-BFFB-E076763E2C7B}" name="USB" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{1C8B55E3-7B48-484B-9DEC-D60D33855BF8}" name="Part Number" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{EB01044E-239A-43EB-B0C2-1F87DDB54160}" name="Description" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}" name="Resistors" displayName="Resistors" ref="A1:H22" totalsRowShown="0" headerRowDxfId="32" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}" name="Resistors" displayName="Resistors" ref="A1:H22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:H22" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H12">
-    <sortCondition ref="C1:C12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
+    <sortCondition ref="C1:C22"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{5CCC4BAB-E9A7-42D2-BFCF-40A14E4FCFB3}" name="Added to Altium?" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{E2BB1AD3-36C9-4D80-8A78-E46D0D28B43D}" name="Resistance" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{C2F2285A-BFA3-4714-8945-6FE63C9CDE81}" name="Res (Raw)" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{5CCC4BAB-E9A7-42D2-BFCF-40A14E4FCFB3}" name="Added to Altium?" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E2BB1AD3-36C9-4D80-8A78-E46D0D28B43D}" name="Resistance" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C2F2285A-BFA3-4714-8945-6FE63C9CDE81}" name="Res (Raw)" dataDxfId="0">
       <calculatedColumnFormula>IF(ISNUMBER(B2),
- B2,
- VALUE(LEFT(B2, LEN(B2)-1)) *
- IF(RIGHT(B2,1)="k",1000,
- IF(RIGHT(B2,1)="M",1000000,
- IF(RIGHT(B2,1)="m",0.001,1))))</calculatedColumnFormula>
+IF(B2=0,"",B2),
+VALUE(LEFT(B2,LEN(B2)-1))*
+IF(RIGHT(B2,1)="k",1000,
+IF(RIGHT(B2,1)="M",1000000,
+IF(RIGHT(B2,1)="m",0.001,1))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{67EED117-D01D-4FE8-BB40-D7D8F55BAB48}" name="Tolerance" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F1269AFE-5CA5-4F00-93B8-6023E945504D}" name="Package" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A4374340-1758-433F-80B6-83ABF6D97E11}" name="Wattage" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{7C53E4E9-C23D-4482-9A46-441AB8A4E1B1}" name="Part Number" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{BD8216A4-1B75-4738-A589-0D33231AD075}" name="Description" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{67EED117-D01D-4FE8-BB40-D7D8F55BAB48}" name="Tolerance" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{F1269AFE-5CA5-4F00-93B8-6023E945504D}" name="Package" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A4374340-1758-433F-80B6-83ABF6D97E11}" name="Wattage" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{7C53E4E9-C23D-4482-9A46-441AB8A4E1B1}" name="Part Number" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BD8216A4-1B75-4738-A589-0D33231AD075}" name="Description" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,7 +1278,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{EA8CC69A-B6DA-4750-BA77-538662D89C27}" name="Switches" displayName="Switches" ref="A1:G11" totalsRowShown="0">
   <autoFilter ref="A1:G11" xr:uid="{EA8CC69A-B6DA-4750-BA77-538662D89C27}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{AC77A4FF-3DCF-4737-ACB4-F75821B19F57}" name="Added to Altium?" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{AC77A4FF-3DCF-4737-ACB4-F75821B19F57}" name="Added to Altium?" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{C868B851-3D2D-4863-96B3-5412E9A862E1}" name="Function"/>
     <tableColumn id="6" xr3:uid="{D6EA3AC7-CEF9-4E2A-800B-297C8C002273}" name="Circuit"/>
     <tableColumn id="2" xr3:uid="{5048C5E7-258E-4EC2-B0BD-C338C4D84C91}" name="Part Number"/>
@@ -1277,7 +1294,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{82CFED5E-627B-4A23-9BFA-C489CEA32F25}" name="Voltage_Regulators" displayName="Voltage_Regulators" ref="A1:H12" totalsRowShown="0">
   <autoFilter ref="A1:H12" xr:uid="{82CFED5E-627B-4A23-9BFA-C489CEA32F25}"/>
   <tableColumns count="8">
-    <tableColumn id="3" xr3:uid="{DD7A1A9A-DE5A-4766-9947-A308E87BA7FD}" name="Added to Altium?" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DD7A1A9A-DE5A-4766-9947-A308E87BA7FD}" name="Added to Altium?" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{7B7659A2-8D22-4954-B10E-C811D8D29B99}" name="Type"/>
     <tableColumn id="7" xr3:uid="{24DD5DAD-1853-4138-AB66-BA5667E60D26}" name="Operation"/>
     <tableColumn id="8" xr3:uid="{C0E1C407-BC33-4018-B09E-15A16329D7C6}" name="Input Voltage"/>
@@ -1329,7 +1346,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}" name="Diodes" displayName="Diodes" ref="A1:G7" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A1:G7" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{373BF80E-AE0E-45C8-9A43-A9D96680B6E9}" name="Added to Altium?" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{373BF80E-AE0E-45C8-9A43-A9D96680B6E9}" name="Added to Altium?" dataDxfId="44"/>
     <tableColumn id="1" xr3:uid="{3176E398-8316-4079-97C6-E10CED1CC775}" name="Type"/>
     <tableColumn id="2" xr3:uid="{DFDAC67A-8333-4623-A218-F2BB6C8E25E6}" name="Breakdown voltage"/>
     <tableColumn id="3" xr3:uid="{3A72F6DE-D147-42DD-9C1C-BA3A3545DE11}" name="Max Forward Current"/>
@@ -1342,25 +1359,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}" name="Table6" displayName="Table6" ref="A1:E11" totalsRowShown="0" headerRowDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}" name="Table6" displayName="Table6" ref="A1:E11" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A1:E11" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{7A1ACCA6-7C12-421C-A8B0-DAF52C5B82F1}" name="Added to Altium?" dataDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{29766E43-A003-4F30-8FBC-98197408FA6D}" name="Part Number" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{9E0E83BD-C619-4B71-B8D8-093D6B07D9D5}" name="Package" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{6C643D04-D582-419C-9C7F-1B57D4315CFE}" name="Resistance" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{67D14711-9F21-4BBC-9182-15BB5F898016}" name="Description" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{7A1ACCA6-7C12-421C-A8B0-DAF52C5B82F1}" name="Added to Altium?" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{29766E43-A003-4F30-8FBC-98197408FA6D}" name="Part Number" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{9E0E83BD-C619-4B71-B8D8-093D6B07D9D5}" name="Package" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{6C643D04-D582-419C-9C7F-1B57D4315CFE}" name="Resistance" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{67D14711-9F21-4BBC-9182-15BB5F898016}" name="Description" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}" name="Fuses" displayName="Fuses" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}" name="Fuses" displayName="Fuses" ref="A1:G10" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A1:G10" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{9030A4FE-0A13-4A65-8271-CB2306DED874}" name="Added to Altium?" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{7A093B6F-93A8-4A04-9A40-8451BE8854E4}" name="Type" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{9030A4FE-0A13-4A65-8271-CB2306DED874}" name="Added to Altium?" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{7A093B6F-93A8-4A04-9A40-8451BE8854E4}" name="Type" dataDxfId="35"/>
     <tableColumn id="1" xr3:uid="{5D9981C8-F221-4013-A9BA-4E5BF3474E5D}" name="Trip Current"/>
     <tableColumn id="2" xr3:uid="{494ED5E9-E1DA-4E76-9EAF-806837FCC14C}" name="Package"/>
     <tableColumn id="3" xr3:uid="{7EDCBE59-D502-4146-84D0-ACB598015CAD}" name="Max Voltage"/>
@@ -1375,8 +1392,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF6FA6FB-E17E-44DE-A790-4DB35B6C38E6}" name="ICs" displayName="ICs" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10" xr:uid="{CF6FA6FB-E17E-44DE-A790-4DB35B6C38E6}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{2DF829CD-290D-41D3-B284-4B22DE33C4AA}" name="Added to Altium?" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{0460994E-DB61-407B-B7D3-3CAA8ED4BC9D}" name="Function" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{2DF829CD-290D-41D3-B284-4B22DE33C4AA}" name="Added to Altium?" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{0460994E-DB61-407B-B7D3-3CAA8ED4BC9D}" name="Function" dataDxfId="33"/>
     <tableColumn id="6" xr3:uid="{F86F95F1-F9FE-4146-B379-63E1029BD91F}" name="Notes"/>
     <tableColumn id="1" xr3:uid="{B62DE98C-40C5-4F02-871A-56E6F423B932}" name="Part Number"/>
     <tableColumn id="3" xr3:uid="{613F07FA-6CA3-413B-A8EC-C111F4721AB4}" name="Description"/>
@@ -1386,14 +1403,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}" name="Inductors" displayName="Inductors" ref="A1:E11" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}" name="Inductors" displayName="Inductors" ref="A1:E11" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="A1:E11" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{67CA846A-F07D-4034-8F63-B4E47CA7F931}" name="Added to Altium?" dataDxfId="25"/>
-    <tableColumn id="1" xr3:uid="{EBC427FC-C649-421F-A511-F4C6E090217A}" name="Inductance" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{57FAF0ED-182E-4A05-89A5-EE5FE9CF2C31}" name="Package" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{5B4ACDCC-FB26-4063-91C8-D6D43ABD7134}" name="Part Number" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{CFE06357-AAEA-49E4-8ED8-14478316C7C8}" name="Description" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{67CA846A-F07D-4034-8F63-B4E47CA7F931}" name="Added to Altium?" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{EBC427FC-C649-421F-A511-F4C6E090217A}" name="Inductance" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{57FAF0ED-182E-4A05-89A5-EE5FE9CF2C31}" name="Package" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5B4ACDCC-FB26-4063-91C8-D6D43ABD7134}" name="Part Number" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{CFE06357-AAEA-49E4-8ED8-14478316C7C8}" name="Description" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1403,10 +1420,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C732A860-4A42-46A7-A5FA-C00091FE4BA3}" name="LEDs" displayName="LEDs" ref="A1:G10" totalsRowShown="0">
   <autoFilter ref="A1:G10" xr:uid="{C732A860-4A42-46A7-A5FA-C00091FE4BA3}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{B2E48D06-BAB0-4133-877E-867AB2EC32E9}" name="Added to Altium?" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{B2E48D06-BAB0-4133-877E-867AB2EC32E9}" name="Added to Altium?" dataDxfId="26"/>
     <tableColumn id="1" xr3:uid="{727DF6C0-6BC9-4CBC-ACBD-F7D7801F3DED}" name="Color"/>
     <tableColumn id="6" xr3:uid="{2F89F121-2031-4E76-8B64-C6BE1AC4E5A7}" name="Mount Type"/>
-    <tableColumn id="2" xr3:uid="{59EEDA5E-A95B-4620-BC5E-79C5C5FB8AFC}" name="Package" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{59EEDA5E-A95B-4620-BC5E-79C5C5FB8AFC}" name="Package" dataDxfId="25"/>
     <tableColumn id="3" xr3:uid="{95A3DF17-FA71-419C-9869-87ACAC774187}" name="Dome"/>
     <tableColumn id="4" xr3:uid="{30ACC022-FAF3-44FA-97E2-DA5C989B54D7}" name="Part Number"/>
     <tableColumn id="5" xr3:uid="{BDED051F-FA40-461B-85BB-40EDC316E70C}" name="Description"/>
@@ -1990,8 +2007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B4EE80-6917-43D6-8B0A-D27EC0A92AF4}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -2033,7 +2050,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
@@ -2047,7 +2064,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2263,15 +2289,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73385E-A93D-4809-A6CB-D5FDE97D6171}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScale="104" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.6328125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" style="3" customWidth="1"/>
     <col min="5" max="5" width="10" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.7265625" style="3" customWidth="1"/>
@@ -2307,531 +2333,586 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16">
+      <c r="A2" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15">
         <v>27</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <f>IF(ISNUMBER(B2),
- B2,
- VALUE(LEFT(B2, LEN(B2)-1)) *
- IF(RIGHT(B2,1)="k",1000,
- IF(RIGHT(B2,1)="M",1000000,
- IF(RIGHT(B2,1)="m",0.001,1))))</f>
+IF(B2=0,"",B2),
+VALUE(LEFT(B2,LEN(B2)-1))*
+IF(RIGHT(B2,1)="k",1000,
+IF(RIGHT(B2,1)="M",1000000,
+IF(RIGHT(B2,1)="m",0.001,1))))</f>
         <v>27</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="16">
+      <c r="A3" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15">
         <v>33</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <f>IF(ISNUMBER(B3),
- B3,
- VALUE(LEFT(B3, LEN(B3)-1)) *
- IF(RIGHT(B3,1)="k",1000,
- IF(RIGHT(B3,1)="M",1000000,
- IF(RIGHT(B3,1)="m",0.001,1))))</f>
+IF(B3=0,"",B3),
+VALUE(LEFT(B3,LEN(B3)-1))*
+IF(RIGHT(B3,1)="k",1000,
+IF(RIGHT(B3,1)="M",1000000,
+IF(RIGHT(B3,1)="m",0.001,1))))</f>
         <v>33</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="A4" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15">
+        <v>100</v>
+      </c>
+      <c r="C4" s="17">
+        <f>IF(ISNUMBER(B4),
+IF(B4=0,"",B4),
+VALUE(LEFT(B4,LEN(B4)-1))*
+IF(RIGHT(B4,1)="k",1000,
+IF(RIGHT(B4,1)="M",1000000,
+IF(RIGHT(B4,1)="m",0.001,1))))</f>
+        <v>100</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15">
         <v>220</v>
       </c>
-      <c r="C4" s="18">
-        <f>IF(ISNUMBER(B4),
- B4,
- VALUE(LEFT(B4, LEN(B4)-1)) *
- IF(RIGHT(B4,1)="k",1000,
- IF(RIGHT(B4,1)="M",1000000,
- IF(RIGHT(B4,1)="m",0.001,1))))</f>
+      <c r="C5" s="17">
+        <f>IF(ISNUMBER(B5),
+IF(B5=0,"",B5),
+VALUE(LEFT(B5,LEN(B5)-1))*
+IF(RIGHT(B5,1)="k",1000,
+IF(RIGHT(B5,1)="M",1000000,
+IF(RIGHT(B5,1)="m",0.001,1))))</f>
         <v>220</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G5" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H5" s="16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B5" s="16">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15">
         <v>220</v>
       </c>
-      <c r="C5" s="18">
-        <f>IF(ISNUMBER(B5),
- B5,
- VALUE(LEFT(B5, LEN(B5)-1)) *
- IF(RIGHT(B5,1)="k",1000,
- IF(RIGHT(B5,1)="M",1000000,
- IF(RIGHT(B5,1)="m",0.001,1))))</f>
+      <c r="C6" s="17">
+        <f>IF(ISNUMBER(B6),
+IF(B6=0,"",B6),
+VALUE(LEFT(B6,LEN(B6)-1))*
+IF(RIGHT(B6,1)="k",1000,
+IF(RIGHT(B6,1)="M",1000000,
+IF(RIGHT(B6,1)="m",0.001,1))))</f>
         <v>220</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B6" s="16" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="18">
-        <f>IF(ISNUMBER(B6),
- B6,
- VALUE(LEFT(B6, LEN(B6)-1)) *
- IF(RIGHT(B6,1)="k",1000,
- IF(RIGHT(B6,1)="M",1000000,
- IF(RIGHT(B6,1)="m",0.001,1))))</f>
+      <c r="C7" s="17">
+        <f>IF(ISNUMBER(B7),
+IF(B7=0,"",B7),
+VALUE(LEFT(B7,LEN(B7)-1))*
+IF(RIGHT(B7,1)="k",1000,
+IF(RIGHT(B7,1)="M",1000000,
+IF(RIGHT(B7,1)="m",0.001,1))))</f>
         <v>1000</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B7" s="16" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="18">
-        <f>IF(ISNUMBER(B7),
- B7,
- VALUE(LEFT(B7, LEN(B7)-1)) *
- IF(RIGHT(B7,1)="k",1000,
- IF(RIGHT(B7,1)="M",1000000,
- IF(RIGHT(B7,1)="m",0.001,1))))</f>
+      <c r="C8" s="17">
+        <f>IF(ISNUMBER(B8),
+IF(B8=0,"",B8),
+VALUE(LEFT(B8,LEN(B8)-1))*
+IF(RIGHT(B8,1)="k",1000,
+IF(RIGHT(B8,1)="M",1000000,
+IF(RIGHT(B8,1)="m",0.001,1))))</f>
         <v>1000</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="16" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="18">
-        <f>IF(ISNUMBER(B8),
- B8,
- VALUE(LEFT(B8, LEN(B8)-1)) *
- IF(RIGHT(B8,1)="k",1000,
- IF(RIGHT(B8,1)="M",1000000,
- IF(RIGHT(B8,1)="m",0.001,1))))</f>
+      <c r="C9" s="17">
+        <f>IF(ISNUMBER(B9),
+IF(B9=0,"",B9),
+VALUE(LEFT(B9,LEN(B9)-1))*
+IF(RIGHT(B9,1)="k",1000,
+IF(RIGHT(B9,1)="M",1000000,
+IF(RIGHT(B9,1)="m",0.001,1))))</f>
         <v>2000</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G9" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H9" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="16" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="18">
-        <f>IF(ISNUMBER(B9),
- B9,
- VALUE(LEFT(B9, LEN(B9)-1)) *
- IF(RIGHT(B9,1)="k",1000,
- IF(RIGHT(B9,1)="M",1000000,
- IF(RIGHT(B9,1)="m",0.001,1))))</f>
+      <c r="C10" s="17">
+        <f>IF(ISNUMBER(B10),
+IF(B10=0,"",B10),
+VALUE(LEFT(B10,LEN(B10)-1))*
+IF(RIGHT(B10,1)="k",1000,
+IF(RIGHT(B10,1)="M",1000000,
+IF(RIGHT(B10,1)="m",0.001,1))))</f>
         <v>5100</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G10" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H10" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="16" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C10" s="18">
-        <f>IF(ISNUMBER(B10),
- B10,
- VALUE(LEFT(B10, LEN(B10)-1)) *
- IF(RIGHT(B10,1)="k",1000,
- IF(RIGHT(B10,1)="M",1000000,
- IF(RIGHT(B10,1)="m",0.001,1))))</f>
+      <c r="C11" s="17">
+        <f>IF(ISNUMBER(B11),
+IF(B11=0,"",B11),
+VALUE(LEFT(B11,LEN(B11)-1))*
+IF(RIGHT(B11,1)="k",1000,
+IF(RIGHT(B11,1)="M",1000000,
+IF(RIGHT(B11,1)="m",0.001,1))))</f>
         <v>10000</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G11" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H11" s="16" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B11" s="16" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="18">
-        <f>IF(ISNUMBER(B11),
- B11,
- VALUE(LEFT(B11, LEN(B11)-1)) *
- IF(RIGHT(B11,1)="k",1000,
- IF(RIGHT(B11,1)="M",1000000,
- IF(RIGHT(B11,1)="m",0.001,1))))</f>
+      <c r="C12" s="17">
+        <f>IF(ISNUMBER(B12),
+IF(B12=0,"",B12),
+VALUE(LEFT(B12,LEN(B12)-1))*
+IF(RIGHT(B12,1)="k",1000,
+IF(RIGHT(B12,1)="M",1000000,
+IF(RIGHT(B12,1)="m",0.001,1))))</f>
         <v>10000</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G12" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H12" s="16" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="16" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="18">
-        <f>IF(ISNUMBER(B12),
- B12,
- VALUE(LEFT(B12, LEN(B12)-1)) *
- IF(RIGHT(B12,1)="k",1000,
- IF(RIGHT(B12,1)="M",1000000,
- IF(RIGHT(B12,1)="m",0.001,1))))</f>
+      <c r="C13" s="17">
+        <f>IF(ISNUMBER(B13),
+IF(B13=0,"",B13),
+VALUE(LEFT(B13,LEN(B13)-1))*
+IF(RIGHT(B13,1)="k",1000,
+IF(RIGHT(B13,1)="M",1000000,
+IF(RIGHT(B13,1)="m",0.001,1))))</f>
         <v>52300</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H13" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B13" s="16">
-        <v>0</v>
-      </c>
-      <c r="C13" s="18">
-        <f t="shared" ref="C13:C22" si="0">IF(ISNUMBER(B13),
- B13,
- VALUE(LEFT(B13, LEN(B13)-1)) *
- IF(RIGHT(B13,1)="k",1000,
- IF(RIGHT(B13,1)="M",1000000,
- IF(RIGHT(B13,1)="m",0.001,1))))</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-    </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B14" s="16">
-        <v>0</v>
-      </c>
-      <c r="C14" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="A14" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" s="15">
+        <v>0</v>
+      </c>
+      <c r="C14" s="17" t="str">
+        <f>IF(ISNUMBER(B14),
+IF(B14=0,"",B14),
+VALUE(LEFT(B14,LEN(B14)-1))*
+IF(RIGHT(B14,1)="k",1000,
+IF(RIGHT(B14,1)="M",1000000,
+IF(RIGHT(B14,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B15" s="16">
-        <v>0</v>
-      </c>
-      <c r="C15" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="A15" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" s="15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="17" t="str">
+        <f>IF(ISNUMBER(B15),
+IF(B15=0,"",B15),
+VALUE(LEFT(B15,LEN(B15)-1))*
+IF(RIGHT(B15,1)="k",1000,
+IF(RIGHT(B15,1)="M",1000000,
+IF(RIGHT(B15,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" s="16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
+      <c r="A16" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" s="15">
+        <v>0</v>
+      </c>
+      <c r="C16" s="17" t="str">
+        <f>IF(ISNUMBER(B16),
+IF(B16=0,"",B16),
+VALUE(LEFT(B16,LEN(B16)-1))*
+IF(RIGHT(B16,1)="k",1000,
+IF(RIGHT(B16,1)="M",1000000,
+IF(RIGHT(B16,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B17" s="16">
-        <v>0</v>
-      </c>
-      <c r="C17" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="A17" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" s="15">
+        <v>0</v>
+      </c>
+      <c r="C17" s="17" t="str">
+        <f>IF(ISNUMBER(B17),
+IF(B17=0,"",B17),
+VALUE(LEFT(B17,LEN(B17)-1))*
+IF(RIGHT(B17,1)="k",1000,
+IF(RIGHT(B17,1)="M",1000000,
+IF(RIGHT(B17,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B18" s="16">
-        <v>0</v>
-      </c>
-      <c r="C18" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="A18" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" s="15">
+        <v>0</v>
+      </c>
+      <c r="C18" s="17" t="str">
+        <f>IF(ISNUMBER(B18),
+IF(B18=0,"",B18),
+VALUE(LEFT(B18,LEN(B18)-1))*
+IF(RIGHT(B18,1)="k",1000,
+IF(RIGHT(B18,1)="M",1000000,
+IF(RIGHT(B18,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B19" s="16">
-        <v>0</v>
-      </c>
-      <c r="C19" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="A19" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" s="15">
+        <v>0</v>
+      </c>
+      <c r="C19" s="17" t="str">
+        <f>IF(ISNUMBER(B19),
+IF(B19=0,"",B19),
+VALUE(LEFT(B19,LEN(B19)-1))*
+IF(RIGHT(B19,1)="k",1000,
+IF(RIGHT(B19,1)="M",1000000,
+IF(RIGHT(B19,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B20" s="16">
-        <v>0</v>
-      </c>
-      <c r="C20" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="A20" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" s="15">
+        <v>0</v>
+      </c>
+      <c r="C20" s="17" t="str">
+        <f>IF(ISNUMBER(B20),
+IF(B20=0,"",B20),
+VALUE(LEFT(B20,LEN(B20)-1))*
+IF(RIGHT(B20,1)="k",1000,
+IF(RIGHT(B20,1)="M",1000000,
+IF(RIGHT(B20,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B21" s="16">
-        <v>0</v>
-      </c>
-      <c r="C21" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="A21" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0</v>
+      </c>
+      <c r="C21" s="17" t="str">
+        <f>IF(ISNUMBER(B21),
+IF(B21=0,"",B21),
+VALUE(LEFT(B21,LEN(B21)-1))*
+IF(RIGHT(B21,1)="k",1000,
+IF(RIGHT(B21,1)="M",1000000,
+IF(RIGHT(B21,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="B22" s="16">
-        <v>0</v>
-      </c>
-      <c r="C22" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
+      <c r="A22" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B22" s="15">
+        <v>0</v>
+      </c>
+      <c r="C22" s="17" t="str">
+        <f>IF(ISNUMBER(B22),
+IF(B22=0,"",B22),
+VALUE(LEFT(B22,LEN(B22)-1))*
+IF(RIGHT(B22,1)="k",1000,
+IF(RIGHT(B22,1)="M",1000000,
+IF(RIGHT(B22,1)="m",0.001,1))))</f>
+        <v/>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4315,6 +4396,7 @@
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="16.90625" customWidth="1"/>
     <col min="7" max="7" width="26.7265625" customWidth="1"/>
+    <col min="8" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
@@ -4438,6 +4520,7 @@
     <col min="2" max="3" width="27.7265625" customWidth="1"/>
     <col min="4" max="4" width="24.90625" customWidth="1"/>
     <col min="5" max="5" width="55.36328125" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
added RS-232 connector for acoustic modems
</commit_message>
<xml_diff>
--- a/Altium Parts.xlsx
+++ b/Altium Parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russe\Repositories\MIL\MIL-Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48AB737-AB46-47AD-B6E2-0727066BB290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C672C54D-8B1D-4360-8B2E-080101130DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="12" xr2:uid="{78817FF2-1CC3-4A74-8C91-2AFFF0842C3F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="2" xr2:uid="{78817FF2-1CC3-4A74-8C91-2AFFF0842C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome!" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="251">
   <si>
     <t>Capacitance</t>
   </si>
@@ -515,9 +515,6 @@
     <t>TB002-500-02BE</t>
   </si>
   <si>
-    <t>Number Pins</t>
-  </si>
-  <si>
     <t>Series / Family</t>
   </si>
   <si>
@@ -792,6 +789,24 @@
   </si>
   <si>
     <t>RES 100 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>D-Sub</t>
+  </si>
+  <si>
+    <t>LD09S33E4GV00LF</t>
+  </si>
+  <si>
+    <t>9 Position D-Sub Receptacle, Female Sockets Connector</t>
+  </si>
+  <si>
+    <t># Pins</t>
+  </si>
+  <si>
+    <t>For RS-232</t>
+  </si>
+  <si>
+    <t>USB2.0-3.1</t>
   </si>
 </sst>
 </file>
@@ -906,7 +921,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="58">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
+          <xfpb:DXFComplement i="0"/>
+        </ext>
+      </extLst>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -918,46 +973,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1116,9 +1137,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1198,13 +1216,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{66640DDE-A600-4D40-886A-D93F6DB5FAB3}" name="Capacitors" displayName="Capacitors" ref="A1:I26" totalsRowShown="0">
   <autoFilter ref="A1:I26" xr:uid="{66640DDE-A600-4D40-886A-D93F6DB5FAB3}"/>
   <tableColumns count="9">
-    <tableColumn id="8" xr3:uid="{B97E7FE0-D68A-4659-9DE5-965B7C74FB58}" name="Added to Altium?" dataDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{B97E7FE0-D68A-4659-9DE5-965B7C74FB58}" name="Added to Altium?" dataDxfId="57"/>
     <tableColumn id="1" xr3:uid="{BDC3005D-8889-49B9-B05B-9B4FB822D92C}" name="Capacitance"/>
     <tableColumn id="2" xr3:uid="{204119AE-0485-4922-A3C8-7CDD048C63F5}" name="Package"/>
     <tableColumn id="3" xr3:uid="{13A5BE24-7E3B-42A7-BB30-CF0EA6F4873D}" name="Max Voltage"/>
     <tableColumn id="4" xr3:uid="{D4BF488D-A80E-4525-A0D1-501D554CEDF7}" name="Tolerance"/>
-    <tableColumn id="5" xr3:uid="{08BCE889-36CA-4A02-9976-7D80BAE9681D}" name="Mounting Type" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{B82114B5-A4D9-4327-9F80-0D9587A64062}" name="Polarity" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{08BCE889-36CA-4A02-9976-7D80BAE9681D}" name="Mounting Type" dataDxfId="56"/>
+    <tableColumn id="9" xr3:uid="{B82114B5-A4D9-4327-9F80-0D9587A64062}" name="Polarity" dataDxfId="55"/>
     <tableColumn id="6" xr3:uid="{31CBAF16-36EA-4251-9AC8-58F6F46900E9}" name="Material"/>
     <tableColumn id="7" xr3:uid="{571D64FC-0F67-4FD0-B071-89D71A56F7C6}" name="Manufacturer Part Number"/>
   </tableColumns>
@@ -1216,7 +1234,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{7B88261C-6B3D-4539-9169-7D9FC231B64A}" name="Misc" displayName="Misc" ref="A1:D13" totalsRowShown="0">
   <autoFilter ref="A1:D13" xr:uid="{7B88261C-6B3D-4539-9169-7D9FC231B64A}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{6C04560D-813B-4E79-B81B-87E653E3F958}" name="Added to Altium?" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{6C04560D-813B-4E79-B81B-87E653E3F958}" name="Added to Altium?" dataDxfId="26"/>
     <tableColumn id="1" xr3:uid="{07652CF2-D7CA-452D-A87D-CEBA35FEC12A}" name="Function"/>
     <tableColumn id="2" xr3:uid="{A9FCB299-A552-4123-B45A-F31F0DC5BB9B}" name="Part Number"/>
     <tableColumn id="3" xr3:uid="{2F50D30B-F60A-4BAF-AE6D-0A3909047904}" name="Description"/>
@@ -1226,37 +1244,37 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9DA4F768-7F47-4563-8367-8C9704917FC2}" name="MCUs" displayName="MCUs" ref="A1:J11" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{9DA4F768-7F47-4563-8367-8C9704917FC2}" name="MCUs" displayName="MCUs" ref="A1:J11" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A1:J11" xr:uid="{9DA4F768-7F47-4563-8367-8C9704917FC2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J11">
     <sortCondition ref="B1:B11"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="7" xr3:uid="{B7904B75-EB47-4AE0-AC16-835BCD406E73}" name="Added to Altium?" dataDxfId="21"/>
-    <tableColumn id="1" xr3:uid="{0881C807-AE0D-4E97-942D-F1BB4BC72740}" name="Name" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{FF11C1E0-268B-4AB9-A529-8334EF2C69FD}" name="# GPIO" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{55162BE7-C291-4B9F-ABE8-A7DE102A5A2F}" name="UART" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{12871EC5-67F1-442C-B9F6-E715FA2B13DA}" name="SPI" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{0676FDA2-81C4-49A9-A3D1-DEE7F28D8014}" name="I2C" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{4D86DECE-60FC-46A0-B57F-AB144D9C1459}" name="PWM" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{F498CA82-C855-4B59-BFFB-E076763E2C7B}" name="USB" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{1C8B55E3-7B48-484B-9DEC-D60D33855BF8}" name="Part Number" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{EB01044E-239A-43EB-B0C2-1F87DDB54160}" name="Description" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{B7904B75-EB47-4AE0-AC16-835BCD406E73}" name="Added to Altium?" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{0881C807-AE0D-4E97-942D-F1BB4BC72740}" name="Name" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{FF11C1E0-268B-4AB9-A529-8334EF2C69FD}" name="# GPIO" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{55162BE7-C291-4B9F-ABE8-A7DE102A5A2F}" name="UART" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{12871EC5-67F1-442C-B9F6-E715FA2B13DA}" name="SPI" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{0676FDA2-81C4-49A9-A3D1-DEE7F28D8014}" name="I2C" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{4D86DECE-60FC-46A0-B57F-AB144D9C1459}" name="PWM" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{F498CA82-C855-4B59-BFFB-E076763E2C7B}" name="USB" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{1C8B55E3-7B48-484B-9DEC-D60D33855BF8}" name="Part Number" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{EB01044E-239A-43EB-B0C2-1F87DDB54160}" name="Description" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}" name="Resistors" displayName="Resistors" ref="A1:H22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}" name="Resistors" displayName="Resistors" ref="A1:H22" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:H22" xr:uid="{FE99B236-7512-4792-AE6E-EED4D7BDA003}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
     <sortCondition ref="C1:C22"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{5CCC4BAB-E9A7-42D2-BFCF-40A14E4FCFB3}" name="Added to Altium?" dataDxfId="1"/>
-    <tableColumn id="1" xr3:uid="{E2BB1AD3-36C9-4D80-8A78-E46D0D28B43D}" name="Resistance" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{C2F2285A-BFA3-4714-8945-6FE63C9CDE81}" name="Res (Raw)" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{5CCC4BAB-E9A7-42D2-BFCF-40A14E4FCFB3}" name="Added to Altium?" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{E2BB1AD3-36C9-4D80-8A78-E46D0D28B43D}" name="Resistance" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{C2F2285A-BFA3-4714-8945-6FE63C9CDE81}" name="Res (Raw)" dataDxfId="9">
       <calculatedColumnFormula>IF(ISNUMBER(B2),
 IF(B2=0,"",B2),
 VALUE(LEFT(B2,LEN(B2)-1))*
@@ -1264,11 +1282,11 @@
 IF(RIGHT(B2,1)="M",1000000,
 IF(RIGHT(B2,1)="m",0.001,1))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{67EED117-D01D-4FE8-BB40-D7D8F55BAB48}" name="Tolerance" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{F1269AFE-5CA5-4F00-93B8-6023E945504D}" name="Package" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A4374340-1758-433F-80B6-83ABF6D97E11}" name="Wattage" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{7C53E4E9-C23D-4482-9A46-441AB8A4E1B1}" name="Part Number" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{BD8216A4-1B75-4738-A589-0D33231AD075}" name="Description" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{67EED117-D01D-4FE8-BB40-D7D8F55BAB48}" name="Tolerance" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{F1269AFE-5CA5-4F00-93B8-6023E945504D}" name="Package" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A4374340-1758-433F-80B6-83ABF6D97E11}" name="Wattage" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{7C53E4E9-C23D-4482-9A46-441AB8A4E1B1}" name="Part Number" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{BD8216A4-1B75-4738-A589-0D33231AD075}" name="Description" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1278,7 +1296,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{EA8CC69A-B6DA-4750-BA77-538662D89C27}" name="Switches" displayName="Switches" ref="A1:G11" totalsRowShown="0">
   <autoFilter ref="A1:G11" xr:uid="{EA8CC69A-B6DA-4750-BA77-538662D89C27}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{AC77A4FF-3DCF-4737-ACB4-F75821B19F57}" name="Added to Altium?" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{AC77A4FF-3DCF-4737-ACB4-F75821B19F57}" name="Added to Altium?" dataDxfId="3"/>
     <tableColumn id="1" xr3:uid="{C868B851-3D2D-4863-96B3-5412E9A862E1}" name="Function"/>
     <tableColumn id="6" xr3:uid="{D6EA3AC7-CEF9-4E2A-800B-297C8C002273}" name="Circuit"/>
     <tableColumn id="2" xr3:uid="{5048C5E7-258E-4EC2-B0BD-C338C4D84C91}" name="Part Number"/>
@@ -1294,7 +1312,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{82CFED5E-627B-4A23-9BFA-C489CEA32F25}" name="Voltage_Regulators" displayName="Voltage_Regulators" ref="A1:H12" totalsRowShown="0">
   <autoFilter ref="A1:H12" xr:uid="{82CFED5E-627B-4A23-9BFA-C489CEA32F25}"/>
   <tableColumns count="8">
-    <tableColumn id="3" xr3:uid="{DD7A1A9A-DE5A-4766-9947-A308E87BA7FD}" name="Added to Altium?" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DD7A1A9A-DE5A-4766-9947-A308E87BA7FD}" name="Added to Altium?" dataDxfId="2"/>
     <tableColumn id="1" xr3:uid="{7B7659A2-8D22-4954-B10E-C811D8D29B99}" name="Type"/>
     <tableColumn id="7" xr3:uid="{24DD5DAD-1853-4138-AB66-BA5667E60D26}" name="Operation"/>
     <tableColumn id="8" xr3:uid="{C0E1C407-BC33-4018-B09E-15A16329D7C6}" name="Input Voltage"/>
@@ -1308,19 +1326,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7090E628-1F8E-4CB3-BC5C-768E76CEFDDC}" name="Connectors" displayName="Connectors" ref="A2:G25" totalsRowShown="0" headerRowDxfId="53">
-  <autoFilter ref="A2:G25" xr:uid="{7090E628-1F8E-4CB3-BC5C-768E76CEFDDC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G24">
-    <sortCondition ref="B2:B25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7090E628-1F8E-4CB3-BC5C-768E76CEFDDC}" name="Connectors" displayName="Connectors" ref="A1:H30" totalsRowShown="0" headerRowDxfId="54">
+  <autoFilter ref="A1:H30" xr:uid="{7090E628-1F8E-4CB3-BC5C-768E76CEFDDC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
+    <sortCondition ref="B1:B30"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{CE9E315A-1702-4F78-8ECF-1DA1A2B792AA}" name="Added to Altium?" dataDxfId="52"/>
-    <tableColumn id="1" xr3:uid="{D5AE5A29-FEF0-4556-97F0-002479587894}" name="Series / Family" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{8673F73F-EA18-4F48-837C-C3D933082CD8}" name="Number Pins" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{F61E1994-58CD-4ECF-A835-1786BECF70C2}" name="Gender (plug/port)" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{ADD992CB-74CD-4839-9C1F-4CA1C98DDDE6}" name="Part Number" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{E04857DF-CEB1-4D64-87C3-2580C252E44F}" name="Description" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{DAAED122-6C39-41BF-BCC4-71CD183DA6BB}" name="Mating Connector Part Number" dataDxfId="46"/>
+  <tableColumns count="8">
+    <tableColumn id="7" xr3:uid="{CE9E315A-1702-4F78-8ECF-1DA1A2B792AA}" name="Added to Altium?" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{D5AE5A29-FEF0-4556-97F0-002479587894}" name="Series / Family" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{8673F73F-EA18-4F48-837C-C3D933082CD8}" name="# Pins" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{F61E1994-58CD-4ECF-A835-1786BECF70C2}" name="Gender (plug/port)" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{ADD992CB-74CD-4839-9C1F-4CA1C98DDDE6}" name="Part Number" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{0052054B-61D9-4444-933B-4830DE18EF5D}" name="Mating Connector Part Number" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{DF57140F-10E9-43CB-BE16-5AB59D2592F7}" name="Notes" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{E04857DF-CEB1-4D64-87C3-2580C252E44F}" name="Description" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1343,10 +1362,10 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}" name="Diodes" displayName="Diodes" ref="A1:G7" totalsRowShown="0" headerRowDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}" name="Diodes" displayName="Diodes" ref="A1:G7" totalsRowShown="0" headerRowDxfId="47">
   <autoFilter ref="A1:G7" xr:uid="{AC1B69C7-59BA-492E-BEF3-378F8F5A5F42}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{373BF80E-AE0E-45C8-9A43-A9D96680B6E9}" name="Added to Altium?" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{373BF80E-AE0E-45C8-9A43-A9D96680B6E9}" name="Added to Altium?" dataDxfId="46"/>
     <tableColumn id="1" xr3:uid="{3176E398-8316-4079-97C6-E10CED1CC775}" name="Type"/>
     <tableColumn id="2" xr3:uid="{DFDAC67A-8333-4623-A218-F2BB6C8E25E6}" name="Breakdown voltage"/>
     <tableColumn id="3" xr3:uid="{3A72F6DE-D147-42DD-9C1C-BA3A3545DE11}" name="Max Forward Current"/>
@@ -1359,25 +1378,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}" name="Table6" displayName="Table6" ref="A1:E11" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}" name="Table6" displayName="Table6" ref="A1:E11" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="A1:E11" xr:uid="{EE7552C4-F486-457F-A2F8-480493B7351C}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{7A1ACCA6-7C12-421C-A8B0-DAF52C5B82F1}" name="Added to Altium?" dataDxfId="42"/>
-    <tableColumn id="1" xr3:uid="{29766E43-A003-4F30-8FBC-98197408FA6D}" name="Part Number" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{9E0E83BD-C619-4B71-B8D8-093D6B07D9D5}" name="Package" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{6C643D04-D582-419C-9C7F-1B57D4315CFE}" name="Resistance" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{67D14711-9F21-4BBC-9182-15BB5F898016}" name="Description" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{7A1ACCA6-7C12-421C-A8B0-DAF52C5B82F1}" name="Added to Altium?" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{29766E43-A003-4F30-8FBC-98197408FA6D}" name="Part Number" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{9E0E83BD-C619-4B71-B8D8-093D6B07D9D5}" name="Package" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{6C643D04-D582-419C-9C7F-1B57D4315CFE}" name="Resistance" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{67D14711-9F21-4BBC-9182-15BB5F898016}" name="Description" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}" name="Fuses" displayName="Fuses" ref="A1:G10" totalsRowShown="0" headerRowDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}" name="Fuses" displayName="Fuses" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A1:G10" xr:uid="{53E52592-BBF3-4884-BA3C-21683DC4F0F1}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{9030A4FE-0A13-4A65-8271-CB2306DED874}" name="Added to Altium?" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{7A093B6F-93A8-4A04-9A40-8451BE8854E4}" name="Type" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{9030A4FE-0A13-4A65-8271-CB2306DED874}" name="Added to Altium?" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{7A093B6F-93A8-4A04-9A40-8451BE8854E4}" name="Type" dataDxfId="37"/>
     <tableColumn id="1" xr3:uid="{5D9981C8-F221-4013-A9BA-4E5BF3474E5D}" name="Trip Current"/>
     <tableColumn id="2" xr3:uid="{494ED5E9-E1DA-4E76-9EAF-806837FCC14C}" name="Package"/>
     <tableColumn id="3" xr3:uid="{7EDCBE59-D502-4146-84D0-ACB598015CAD}" name="Max Voltage"/>
@@ -1392,8 +1411,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{CF6FA6FB-E17E-44DE-A790-4DB35B6C38E6}" name="ICs" displayName="ICs" ref="A1:E10" totalsRowShown="0">
   <autoFilter ref="A1:E10" xr:uid="{CF6FA6FB-E17E-44DE-A790-4DB35B6C38E6}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{2DF829CD-290D-41D3-B284-4B22DE33C4AA}" name="Added to Altium?" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{0460994E-DB61-407B-B7D3-3CAA8ED4BC9D}" name="Function" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{2DF829CD-290D-41D3-B284-4B22DE33C4AA}" name="Added to Altium?" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{0460994E-DB61-407B-B7D3-3CAA8ED4BC9D}" name="Function" dataDxfId="35"/>
     <tableColumn id="6" xr3:uid="{F86F95F1-F9FE-4146-B379-63E1029BD91F}" name="Notes"/>
     <tableColumn id="1" xr3:uid="{B62DE98C-40C5-4F02-871A-56E6F423B932}" name="Part Number"/>
     <tableColumn id="3" xr3:uid="{613F07FA-6CA3-413B-A8EC-C111F4721AB4}" name="Description"/>
@@ -1403,14 +1422,14 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}" name="Inductors" displayName="Inductors" ref="A1:E11" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}" name="Inductors" displayName="Inductors" ref="A1:E11" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A1:E11" xr:uid="{8788865D-3714-4394-BD76-99FF24EF6888}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{67CA846A-F07D-4034-8F63-B4E47CA7F931}" name="Added to Altium?" dataDxfId="31"/>
-    <tableColumn id="1" xr3:uid="{EBC427FC-C649-421F-A511-F4C6E090217A}" name="Inductance" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{57FAF0ED-182E-4A05-89A5-EE5FE9CF2C31}" name="Package" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{5B4ACDCC-FB26-4063-91C8-D6D43ABD7134}" name="Part Number" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{CFE06357-AAEA-49E4-8ED8-14478316C7C8}" name="Description" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{67CA846A-F07D-4034-8F63-B4E47CA7F931}" name="Added to Altium?" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{EBC427FC-C649-421F-A511-F4C6E090217A}" name="Inductance" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{57FAF0ED-182E-4A05-89A5-EE5FE9CF2C31}" name="Package" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{5B4ACDCC-FB26-4063-91C8-D6D43ABD7134}" name="Part Number" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{CFE06357-AAEA-49E4-8ED8-14478316C7C8}" name="Description" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1420,10 +1439,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{C732A860-4A42-46A7-A5FA-C00091FE4BA3}" name="LEDs" displayName="LEDs" ref="A1:G10" totalsRowShown="0">
   <autoFilter ref="A1:G10" xr:uid="{C732A860-4A42-46A7-A5FA-C00091FE4BA3}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{B2E48D06-BAB0-4133-877E-867AB2EC32E9}" name="Added to Altium?" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{B2E48D06-BAB0-4133-877E-867AB2EC32E9}" name="Added to Altium?" dataDxfId="28"/>
     <tableColumn id="1" xr3:uid="{727DF6C0-6BC9-4CBC-ACBD-F7D7801F3DED}" name="Color"/>
     <tableColumn id="6" xr3:uid="{2F89F121-2031-4E76-8B64-C6BE1AC4E5A7}" name="Mount Type"/>
-    <tableColumn id="2" xr3:uid="{59EEDA5E-A95B-4620-BC5E-79C5C5FB8AFC}" name="Package" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{59EEDA5E-A95B-4620-BC5E-79C5C5FB8AFC}" name="Package" dataDxfId="27"/>
     <tableColumn id="3" xr3:uid="{95A3DF17-FA71-419C-9869-87ACAC774187}" name="Dome"/>
     <tableColumn id="4" xr3:uid="{30ACC022-FAF3-44FA-97E2-DA5C989B54D7}" name="Part Number"/>
     <tableColumn id="5" xr3:uid="{BDED051F-FA40-461B-85BB-40EDC316E70C}" name="Description"/>
@@ -1762,83 +1781,83 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1868,13 +1887,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
@@ -2022,7 +2041,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>82</v>
@@ -2039,13 +2058,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" t="s">
         <v>239</v>
-      </c>
-      <c r="C2" t="s">
-        <v>209</v>
-      </c>
-      <c r="D2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2067,13 +2086,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C4" t="s">
         <v>241</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>242</v>
-      </c>
-      <c r="D4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -2149,28 +2168,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>226</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>228</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>2</v>
@@ -2184,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C2" s="14">
         <v>30</v>
@@ -2205,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -2289,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73385E-A93D-4809-A6CB-D5FDE97D6171}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+    <sheetView zoomScale="104" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2308,13 +2327,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>51</v>
@@ -2340,7 +2359,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="17">
-        <f>IF(ISNUMBER(B2),
+        <f t="shared" ref="C2:C22" si="0">IF(ISNUMBER(B2),
 IF(B2=0,"",B2),
 VALUE(LEFT(B2,LEN(B2)-1))*
 IF(RIGHT(B2,1)="k",1000,
@@ -2355,7 +2374,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>57</v>
@@ -2372,12 +2391,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="17">
-        <f>IF(ISNUMBER(B3),
-IF(B3=0,"",B3),
-VALUE(LEFT(B3,LEN(B3)-1))*
-IF(RIGHT(B3,1)="k",1000,
-IF(RIGHT(B3,1)="M",1000000,
-IF(RIGHT(B3,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -2404,12 +2418,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="17">
-        <f>IF(ISNUMBER(B4),
-IF(B4=0,"",B4),
-VALUE(LEFT(B4,LEN(B4)-1))*
-IF(RIGHT(B4,1)="k",1000,
-IF(RIGHT(B4,1)="M",1000000,
-IF(RIGHT(B4,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -2419,13 +2428,13 @@
         <v>9</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G4" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="H4" s="16" t="s">
         <v>244</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -2436,12 +2445,7 @@
         <v>220</v>
       </c>
       <c r="C5" s="17">
-        <f>IF(ISNUMBER(B5),
-IF(B5=0,"",B5),
-VALUE(LEFT(B5,LEN(B5)-1))*
-IF(RIGHT(B5,1)="k",1000,
-IF(RIGHT(B5,1)="M",1000000,
-IF(RIGHT(B5,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>220</v>
       </c>
       <c r="D5" s="16" t="s">
@@ -2451,7 +2455,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>63</v>
@@ -2468,12 +2472,7 @@
         <v>220</v>
       </c>
       <c r="C6" s="17">
-        <f>IF(ISNUMBER(B6),
-IF(B6=0,"",B6),
-VALUE(LEFT(B6,LEN(B6)-1))*
-IF(RIGHT(B6,1)="k",1000,
-IF(RIGHT(B6,1)="M",1000000,
-IF(RIGHT(B6,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>220</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -2486,10 +2485,10 @@
         <v>141</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -2500,12 +2499,7 @@
         <v>61</v>
       </c>
       <c r="C7" s="17">
-        <f>IF(ISNUMBER(B7),
-IF(B7=0,"",B7),
-VALUE(LEFT(B7,LEN(B7)-1))*
-IF(RIGHT(B7,1)="k",1000,
-IF(RIGHT(B7,1)="M",1000000,
-IF(RIGHT(B7,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -2515,7 +2509,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>59</v>
@@ -2532,12 +2526,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="17">
-        <f>IF(ISNUMBER(B8),
-IF(B8=0,"",B8),
-VALUE(LEFT(B8,LEN(B8)-1))*
-IF(RIGHT(B8,1)="k",1000,
-IF(RIGHT(B8,1)="M",1000000,
-IF(RIGHT(B8,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -2547,7 +2536,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>134</v>
@@ -2564,12 +2553,7 @@
         <v>70</v>
       </c>
       <c r="C9" s="17">
-        <f>IF(ISNUMBER(B9),
-IF(B9=0,"",B9),
-VALUE(LEFT(B9,LEN(B9)-1))*
-IF(RIGHT(B9,1)="k",1000,
-IF(RIGHT(B9,1)="M",1000000,
-IF(RIGHT(B9,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -2579,7 +2563,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>68</v>
@@ -2596,12 +2580,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="17">
-        <f>IF(ISNUMBER(B10),
-IF(B10=0,"",B10),
-VALUE(LEFT(B10,LEN(B10)-1))*
-IF(RIGHT(B10,1)="k",1000,
-IF(RIGHT(B10,1)="M",1000000,
-IF(RIGHT(B10,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>5100</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -2611,7 +2590,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>55</v>
@@ -2628,12 +2607,7 @@
         <v>139</v>
       </c>
       <c r="C11" s="17">
-        <f>IF(ISNUMBER(B11),
-IF(B11=0,"",B11),
-VALUE(LEFT(B11,LEN(B11)-1))*
-IF(RIGHT(B11,1)="k",1000,
-IF(RIGHT(B11,1)="M",1000000,
-IF(RIGHT(B11,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -2660,12 +2634,7 @@
         <v>139</v>
       </c>
       <c r="C12" s="17">
-        <f>IF(ISNUMBER(B12),
-IF(B12=0,"",B12),
-VALUE(LEFT(B12,LEN(B12)-1))*
-IF(RIGHT(B12,1)="k",1000,
-IF(RIGHT(B12,1)="M",1000000,
-IF(RIGHT(B12,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -2675,13 +2644,13 @@
         <v>9</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -2692,12 +2661,7 @@
         <v>144</v>
       </c>
       <c r="C13" s="17">
-        <f>IF(ISNUMBER(B13),
-IF(B13=0,"",B13),
-VALUE(LEFT(B13,LEN(B13)-1))*
-IF(RIGHT(B13,1)="k",1000,
-IF(RIGHT(B13,1)="M",1000000,
-IF(RIGHT(B13,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v>52300</v>
       </c>
       <c r="D13" s="16" t="s">
@@ -2724,12 +2688,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="17" t="str">
-        <f>IF(ISNUMBER(B14),
-IF(B14=0,"",B14),
-VALUE(LEFT(B14,LEN(B14)-1))*
-IF(RIGHT(B14,1)="k",1000,
-IF(RIGHT(B14,1)="M",1000000,
-IF(RIGHT(B14,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D14" s="16"/>
@@ -2746,12 +2705,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="17" t="str">
-        <f>IF(ISNUMBER(B15),
-IF(B15=0,"",B15),
-VALUE(LEFT(B15,LEN(B15)-1))*
-IF(RIGHT(B15,1)="k",1000,
-IF(RIGHT(B15,1)="M",1000000,
-IF(RIGHT(B15,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D15" s="16"/>
@@ -2768,12 +2722,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="17" t="str">
-        <f>IF(ISNUMBER(B16),
-IF(B16=0,"",B16),
-VALUE(LEFT(B16,LEN(B16)-1))*
-IF(RIGHT(B16,1)="k",1000,
-IF(RIGHT(B16,1)="M",1000000,
-IF(RIGHT(B16,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D16" s="16"/>
@@ -2790,12 +2739,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="17" t="str">
-        <f>IF(ISNUMBER(B17),
-IF(B17=0,"",B17),
-VALUE(LEFT(B17,LEN(B17)-1))*
-IF(RIGHT(B17,1)="k",1000,
-IF(RIGHT(B17,1)="M",1000000,
-IF(RIGHT(B17,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D17" s="16"/>
@@ -2812,12 +2756,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="17" t="str">
-        <f>IF(ISNUMBER(B18),
-IF(B18=0,"",B18),
-VALUE(LEFT(B18,LEN(B18)-1))*
-IF(RIGHT(B18,1)="k",1000,
-IF(RIGHT(B18,1)="M",1000000,
-IF(RIGHT(B18,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D18" s="16"/>
@@ -2834,12 +2773,7 @@
         <v>0</v>
       </c>
       <c r="C19" s="17" t="str">
-        <f>IF(ISNUMBER(B19),
-IF(B19=0,"",B19),
-VALUE(LEFT(B19,LEN(B19)-1))*
-IF(RIGHT(B19,1)="k",1000,
-IF(RIGHT(B19,1)="M",1000000,
-IF(RIGHT(B19,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D19" s="16"/>
@@ -2856,12 +2790,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="17" t="str">
-        <f>IF(ISNUMBER(B20),
-IF(B20=0,"",B20),
-VALUE(LEFT(B20,LEN(B20)-1))*
-IF(RIGHT(B20,1)="k",1000,
-IF(RIGHT(B20,1)="M",1000000,
-IF(RIGHT(B20,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D20" s="16"/>
@@ -2878,12 +2807,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="17" t="str">
-        <f>IF(ISNUMBER(B21),
-IF(B21=0,"",B21),
-VALUE(LEFT(B21,LEN(B21)-1))*
-IF(RIGHT(B21,1)="k",1000,
-IF(RIGHT(B21,1)="M",1000000,
-IF(RIGHT(B21,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D21" s="16"/>
@@ -2900,12 +2824,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="17" t="str">
-        <f>IF(ISNUMBER(B22),
-IF(B22=0,"",B22),
-VALUE(LEFT(B22,LEN(B22)-1))*
-IF(RIGHT(B22,1)="k",1000,
-IF(RIGHT(B22,1)="M",1000000,
-IF(RIGHT(B22,1)="m",0.001,1))))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="D22" s="16"/>
@@ -2944,7 +2863,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>82</v>
@@ -2970,7 +2889,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
         <v>76</v>
@@ -3063,16 +2982,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>87</v>
       </c>
       <c r="C1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E1" t="s">
         <v>89</v>
@@ -3095,10 +3014,10 @@
         <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E2" t="s">
         <v>90</v>
@@ -3110,7 +3029,7 @@
         <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -3121,10 +3040,10 @@
         <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E3" t="s">
         <v>150</v>
@@ -3214,7 +3133,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3229,10 +3148,10 @@
         <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -3261,7 +3180,7 @@
         <v>107</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -3290,7 +3209,7 @@
         <v>107</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -3319,7 +3238,7 @@
         <v>107</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -3348,7 +3267,7 @@
         <v>107</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -3377,7 +3296,7 @@
         <v>107</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
@@ -3406,7 +3325,7 @@
         <v>107</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H7" t="s">
         <v>10</v>
@@ -3435,7 +3354,7 @@
         <v>107</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H8" t="s">
         <v>10</v>
@@ -3464,7 +3383,7 @@
         <v>107</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H9" t="s">
         <v>116</v>
@@ -3569,426 +3488,484 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31311A32-7C4D-4571-8105-957397FF3475}">
-  <dimension ref="A2:XDV27"/>
+  <dimension ref="A1:XDX30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="83" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="113" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.1796875" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="11" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="11" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" customWidth="1"/>
     <col min="5" max="5" width="16.54296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.7265625" style="3" customWidth="1"/>
-    <col min="8" max="16339" width="8.7265625" style="3" hidden="1"/>
-    <col min="16340" max="16340" width="0" style="3" hidden="1"/>
-    <col min="16341" max="16349" width="8.7265625" style="3" hidden="1"/>
-    <col min="16350" max="16350" width="0" style="3" hidden="1"/>
-    <col min="16351" max="16384" width="8.7265625" style="3" hidden="1"/>
+    <col min="6" max="6" width="17" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="37.54296875" style="3" customWidth="1"/>
+    <col min="9" max="16340" width="8.7265625" style="3" hidden="1"/>
+    <col min="16341" max="16341" width="0" style="3" hidden="1"/>
+    <col min="16342" max="16350" width="8.7265625" style="3" hidden="1"/>
+    <col min="16351" max="16352" width="0" style="3" hidden="1"/>
+    <col min="16353" max="16384" width="8.7265625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>204</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="b">
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>153</v>
+        <v>207</v>
+      </c>
+      <c r="C2" s="12">
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="12">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" s="12">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="F3" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="C4" s="12">
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5" s="12">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" s="12">
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" s="12">
         <v>4</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" s="12">
         <v>5</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="12">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" s="12">
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" s="12">
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C12" s="12">
         <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="12">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="G13" s="3" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C14" s="12">
         <v>6</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C15" s="12">
         <v>10</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" s="12">
         <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" s="12">
         <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="12">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="12">
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C20" s="12">
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C21" s="12">
         <v>6</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" s="12">
         <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="b">
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C24" s="12"/>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="b">
         <v>0</v>
       </c>
       <c r="C25" s="12"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="12"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4020,7 +3997,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>100</v>
@@ -4072,19 +4049,19 @@
         <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
         <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -4183,7 +4160,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>87</v>
@@ -4229,22 +4206,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" t="s">
         <v>176</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>177</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>178</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>179</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>180</v>
-      </c>
-      <c r="G3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -4295,7 +4272,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -4324,7 +4301,7 @@
         <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -4402,7 +4379,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>87</v>
@@ -4526,13 +4503,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" t="s">
         <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -4549,7 +4526,7 @@
         <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
         <v>80</v>
@@ -4563,10 +4540,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D3" t="s">
         <v>94</v>
@@ -4580,13 +4557,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" t="s">
         <v>174</v>
-      </c>
-      <c r="E4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -4647,7 +4624,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>47</v>
@@ -4670,7 +4647,7 @@
         <v>48</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>50</v>
@@ -4687,7 +4664,7 @@
         <v>133</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>131</v>

</xml_diff>